<commit_message>
Exact Match Root Logic Added
</commit_message>
<xml_diff>
--- a/matched_data.xlsx
+++ b/matched_data.xlsx
@@ -440,16 +440,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pluszkereset.com</t>
+          <t>elsotano.org</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://h2bet.org</t>
+          <t>https://markets.financialcontent.com/1discountbrokerage/article/getfeatured-2023-8-18-choose-pure-airways-duct-cleaning-dallas-for-unrivaled-quality-and-expertise</t>
         </is>
       </c>
     </row>

</xml_diff>